<commit_message>
redmine #9138 cal sheets for CP02PMUO multiple deployments changed/added.
</commit_message>
<xml_diff>
--- a/CP02PMUO/Omaha_Cal_Info_CP02PMUO_00001.xlsx
+++ b/CP02PMUO/Omaha_Cal_Info_CP02PMUO_00001.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14055" windowHeight="5580" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="8400" yWindow="8900" windowWidth="24720" windowHeight="9820" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$33</definedName>
-    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$35</definedName>
+    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$35</definedName>
     <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0">Moorings!$A$1:$J$94</definedName>
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
@@ -25,17 +25,22 @@
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$404</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$33</definedName>
+    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$35</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$94</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$404</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
   <si>
     <t>Ref Des</t>
   </si>
@@ -161,9 +166,6 @@
   </si>
   <si>
     <t>CP02PMUO-SBS01-01-MOPAK0000</t>
-  </si>
-  <si>
-    <t>CP02PMUO-RII01-02-ADCPTL000</t>
   </si>
   <si>
     <t>CP02PMUO-00001</t>
@@ -246,13 +248,7 @@
     <t>This serial number is a placekeeper used until the correct serial number is found or defined</t>
   </si>
   <si>
-    <t>CP02PMUO-SBS01-00-RTE000000</t>
-  </si>
-  <si>
     <t>CP02PMUO-WFP01-00-WFPENG000</t>
-  </si>
-  <si>
-    <t>PMUO-00001-STC</t>
   </si>
   <si>
     <t>PMUO-00001-MOPAK</t>
@@ -294,6 +290,29 @@
       <t>-VEL3DK000</t>
     </r>
   </si>
+  <si>
+    <t>Recovered after deployment due to failed WFP</t>
+  </si>
+  <si>
+    <r>
+      <t>CP02PMUO-RII01-02-ADCPTL0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <t>units = mm</t>
+  </si>
+  <si>
+    <t>SWE 0005-G</t>
+  </si>
 </sst>
 </file>
 
@@ -302,7 +321,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -395,8 +414,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +458,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,11 +531,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -553,9 +615,29 @@
     <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="12">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,28 +1010,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="39.42578125"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125"/>
-    <col min="7" max="7" width="18.7109375"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="36.140625" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="51" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,12 +1061,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
@@ -1004,26 +1081,22 @@
         <v>41603</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="I2" s="5">
         <v>445</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="15">
-        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>39.941571666666668</v>
-      </c>
-      <c r="M2" s="15">
-        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.779708333333332</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13">
       <c r="D3" s="9"/>
@@ -1035,35 +1108,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125"/>
-    <col min="9" max="9" width="11.85546875"/>
-    <col min="10" max="10" width="14.42578125"/>
-    <col min="11" max="11" width="13.42578125"/>
-    <col min="12" max="1026" width="8.7109375"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,10 +1158,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="17" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="18">
         <v>1</v>
@@ -1099,19 +1172,21 @@
       <c r="E2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="19">
-        <v>427.37</v>
-      </c>
-      <c r="G2" s="17"/>
+      <c r="F2" s="28">
+        <v>425000</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>70</v>
+      </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="17" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="18">
         <v>1</v>
@@ -1131,10 +1206,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="17" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="18">
         <v>1</v>
@@ -1165,58 +1240,35 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="18">
         <v>1</v>
       </c>
-      <c r="D6" s="20">
-        <v>2397</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="21">
-        <v>-820.6</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="D6" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="25" t="s">
         <v>60</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="18">
-        <v>1</v>
-      </c>
-      <c r="D7" s="20">
-        <v>2397</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="19">
-        <v>39.941571666666668</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="8"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="18">
         <v>1</v>
@@ -1225,12 +1277,14 @@
         <v>2397</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="19">
-        <v>-70.779708333333332</v>
-      </c>
-      <c r="G8" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="F8" s="21">
+        <v>-820.6</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
     </row>
@@ -1239,7 +1293,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="18">
         <v>1</v>
@@ -1248,14 +1302,12 @@
         <v>2397</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="21">
-        <v>2.6937E-4</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>48</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F9" s="19">
+        <v>39.941571666666668</v>
+      </c>
+      <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
@@ -1264,7 +1316,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="18">
         <v>1</v>
@@ -1273,14 +1325,12 @@
         <v>2397</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="21">
-        <v>-3.8349E-3</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>49</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F10" s="19">
+        <v>-70.779708333333332</v>
+      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
     </row>
@@ -1289,7 +1339,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="18">
         <v>1</v>
@@ -1298,13 +1348,13 @@
         <v>2397</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F11" s="21">
-        <v>1.771E-4</v>
+        <v>2.6937E-4</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -1314,7 +1364,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="18">
         <v>1</v>
@@ -1323,13 +1373,13 @@
         <v>2397</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="21">
-        <v>-2.7945999999999999E-6</v>
+        <v>-3.8349E-3</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -1339,7 +1389,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="18">
         <v>1</v>
@@ -1348,189 +1398,189 @@
         <v>2397</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" s="21">
-        <v>3.5999999999999997E-2</v>
+        <v>1.771E-4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20">
+        <v>2397</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="21">
+        <v>-2.7945999999999999E-6</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="18">
         <v>1</v>
       </c>
-      <c r="D15" s="18">
-        <v>106</v>
+      <c r="D15" s="20">
+        <v>2397</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="19">
-        <v>39.941571666666668</v>
-      </c>
-      <c r="G15" s="17"/>
+        <v>22</v>
+      </c>
+      <c r="F15" s="21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="18">
-        <v>1</v>
-      </c>
-      <c r="D16" s="18">
-        <v>106</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="19">
-        <v>-70.779708333333332</v>
-      </c>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="19"/>
+      <c r="A17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1</v>
+      </c>
+      <c r="D17" s="18">
+        <v>106</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="19">
+        <v>39.941571666666668</v>
+      </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="17" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="18">
         <v>1</v>
       </c>
-      <c r="D18" s="20">
-        <v>41</v>
+      <c r="D18" s="18">
+        <v>106</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F18" s="19">
-        <v>39.941571666666668</v>
+        <v>-70.779708333333332</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="18">
-        <v>1</v>
-      </c>
-      <c r="D19" s="20">
-        <v>41</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="19">
-        <v>-70.779708333333332</v>
-      </c>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="19"/>
+      <c r="A20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20">
+        <v>41</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="19">
+        <v>39.941571666666668</v>
+      </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="17" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="18">
         <v>1</v>
       </c>
-      <c r="D21" s="18">
-        <v>969</v>
+      <c r="D21" s="20">
+        <v>41</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="F21" s="19">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>35</v>
-      </c>
+        <v>-70.779708333333332</v>
+      </c>
+      <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="18">
-        <v>1</v>
-      </c>
-      <c r="D22" s="18">
-        <v>969</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="19">
-        <v>53</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>53</v>
-      </c>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
@@ -1539,7 +1589,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="18">
         <v>1</v>
@@ -1548,13 +1598,13 @@
         <v>969</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="19">
-        <v>52</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -1564,7 +1614,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="18">
         <v>1</v>
@@ -1573,13 +1623,13 @@
         <v>969</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F24" s="19">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -1589,7 +1639,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="18">
         <v>1</v>
@@ -1598,13 +1648,13 @@
         <v>969</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="F25" s="19">
-        <v>3.9E-2</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>35</v>
+        <v>52</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
@@ -1614,7 +1664,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="18">
         <v>1</v>
@@ -1623,13 +1673,13 @@
         <v>969</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="F26" s="19">
-        <v>700</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
@@ -1639,7 +1689,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="18">
         <v>1</v>
@@ -1648,13 +1698,13 @@
         <v>969</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="19">
-        <v>9.11E-2</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>54</v>
+        <v>64</v>
+      </c>
+      <c r="F27" s="29">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
@@ -1664,7 +1714,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="18">
         <v>1</v>
@@ -1673,13 +1723,13 @@
         <v>969</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="19">
-        <v>1.21E-2</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="F28" s="29">
+        <v>700</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
@@ -1689,7 +1739,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="18">
         <v>1</v>
@@ -1698,13 +1748,13 @@
         <v>969</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="22">
-        <v>3.3560000000000001E-6</v>
+        <v>28</v>
+      </c>
+      <c r="F29" s="19">
+        <v>9.11E-2</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
@@ -1714,7 +1764,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="18">
         <v>1</v>
@@ -1723,141 +1773,151 @@
         <v>969</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="F30" s="19">
-        <v>124</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>35</v>
+        <v>1.21E-2</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="17"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="17"/>
+      <c r="A31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="18">
+        <v>1</v>
+      </c>
+      <c r="D31" s="18">
+        <v>969</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="22">
+        <v>3.3560000000000001E-6</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="18">
         <v>1</v>
       </c>
       <c r="D32" s="18">
-        <v>20423</v>
+        <v>969</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="19">
-        <v>1.2</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>58</v>
+        <v>66</v>
+      </c>
+      <c r="F32" s="29">
+        <v>124</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="18">
-        <v>1</v>
-      </c>
-      <c r="D33" s="18">
-        <v>20423</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="22">
-        <v>9.9599999999999994E-18</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="17"/>
+      <c r="A34" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="18">
+        <v>1</v>
+      </c>
+      <c r="D34" s="18">
+        <v>20423</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="17" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="18">
         <v>1</v>
       </c>
-      <c r="D35" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="25" t="s">
-        <v>61</v>
+      <c r="D35" s="18">
+        <v>20423</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="22">
+        <v>9.9599999999999994E-18</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="18">
-        <v>1</v>
-      </c>
-      <c r="D36" s="18">
-        <v>950</v>
-      </c>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="25"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="18">
         <v>1</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
@@ -1865,33 +1925,45 @@
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="18">
-        <v>1</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-    </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="8"/>
-      <c r="D39" s="16"/>
+      <c r="A39" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CP02PMUO cal and ingest sheet changes
Deleted bogus files and templates
Corrected ADCP reference designators in both cal and ingest sheets
CReated INgest sheet for dep 5
</commit_message>
<xml_diff>
--- a/CP02PMUO/Omaha_Cal_Info_CP02PMUO_00001.xlsx
+++ b/CP02PMUO/Omaha_Cal_Info_CP02PMUO_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="8900" windowWidth="24720" windowHeight="9820" tabRatio="377"/>
+    <workbookView xWindow="8400" yWindow="8895" windowWidth="24720" windowHeight="9825" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -294,24 +294,25 @@
     <t>Recovered after deployment due to failed WFP</t>
   </si>
   <si>
+    <t>units = mm</t>
+  </si>
+  <si>
+    <t>SWE 0005-G</t>
+  </si>
+  <si>
     <r>
-      <t>CP02PMUO-RII01-02-ADCPTL0</t>
+      <t>CP02PMUO-RII01-02-ADCPSL0</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF0000FF"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>10</t>
     </r>
-  </si>
-  <si>
-    <t>units = mm</t>
-  </si>
-  <si>
-    <t>SWE 0005-G</t>
   </si>
 </sst>
 </file>
@@ -321,7 +322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -418,6 +419,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -440,6 +442,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1010,23 +1013,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="10" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="10" width="24.7109375" customWidth="1"/>
     <col min="11" max="11" width="51" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15">
+    <row r="2" spans="1:13">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -1121,22 +1124,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>42</v>
@@ -1176,14 +1179,14 @@
         <v>425000</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>42</v>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -1259,7 +1262,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9">
       <c r="A7" s="8"/>
       <c r="D7" s="16"/>
     </row>
@@ -1936,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="23"/>

</xml_diff>